<commit_message>
Add files to PolarIs-Individual-Corpora-Pathos
</commit_message>
<xml_diff>
--- a/PolarIs-Individual-Corpora/PolarIs-Individual-Corpora-Pathos/PolarIs-2-Pathos.xlsx
+++ b/PolarIs-Individual-Corpora/PolarIs-Individual-Corpora-Pathos/PolarIs-2-Pathos.xlsx
@@ -461,12 +461,12 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Positive_pathos</t>
+          <t>Positive</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>Negative_pathos</t>
+          <t>Negative</t>
         </is>
       </c>
     </row>
@@ -3320,7 +3320,7 @@
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>Anything less gives us more disease, disability, &amp;amp; deaths, esp for the vulnerable groups.</t>
+          <t>Anything less gives us more disease, disability, &amp; deaths, esp for the vulnerable groups.</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
@@ -3349,7 +3349,7 @@
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>@drajm I'm starting to feel a little broken by the failure of Gov/people to undertake basic protections for themselves &amp;amp; others (either by way of ignorance, or selfishness).</t>
+          <t>@drajm I'm starting to feel a little broken by the failure of Gov/people to undertake basic protections for themselves &amp; others (either by way of ignorance, or selfishness).</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
@@ -5700,7 +5700,7 @@
       </c>
       <c r="B182" t="inlineStr">
         <is>
-          <t>I didn’t get it bad but it was still way worse then any cold I’ve ever had and had me out of work for a week &amp;amp; my fiancé legit almost had to go to the hospital &amp;amp; almost lost her job.</t>
+          <t>I didn’t get it bad but it was still way worse then any cold I’ve ever had and had me out of work for a week &amp; my fiancé legit almost had to go to the hospital &amp; almost lost her job.</t>
         </is>
       </c>
       <c r="C182" t="inlineStr">
@@ -7382,7 +7382,7 @@
       </c>
       <c r="B240" t="inlineStr">
         <is>
-          <t>@derby_kira @deadlabrador1 Kira, he initially complimented Trump, &amp;amp; said that he's been a supporter of his.</t>
+          <t>@derby_kira @deadlabrador1 Kira, he initially complimented Trump, &amp; said that he's been a supporter of his.</t>
         </is>
       </c>
       <c r="C240" t="inlineStr">
@@ -7440,7 +7440,7 @@
       </c>
       <c r="B242" t="inlineStr">
         <is>
-          <t>That's the one thing that Alex Jones is calling him out for, &amp;amp; he's absolutely right to do so</t>
+          <t>That's the one thing that Alex Jones is calling him out for, &amp; he's absolutely right to do so</t>
         </is>
       </c>
       <c r="C242" t="inlineStr">
@@ -8546,7 +8546,7 @@
       </c>
       <c r="B280" t="inlineStr">
         <is>
-          <t>@AnnaWhateley We followed the instructions &amp;amp; guidance linked on https://t.co/yFwfsQiaPe for how to isolate in a shared living space.</t>
+          <t>@AnnaWhateley We followed the instructions &amp; guidance linked on https://t.co/yFwfsQiaPe for how to isolate in a shared living space.</t>
         </is>
       </c>
       <c r="C280" t="inlineStr">
@@ -8691,7 +8691,7 @@
       </c>
       <c r="B285" t="inlineStr">
         <is>
-          <t>Kept windows open &amp;amp; cleaned anything they touched.</t>
+          <t>Kept windows open &amp; cleaned anything they touched.</t>
         </is>
       </c>
       <c r="C285" t="inlineStr">
@@ -8720,7 +8720,7 @@
       </c>
       <c r="B286" t="inlineStr">
         <is>
-          <t>Kids isolated in their room &amp;amp; we have a separate bathroom &amp;amp; toilet just for covid positive ppl.</t>
+          <t>Kids isolated in their room &amp; we have a separate bathroom &amp; toilet just for covid positive ppl.</t>
         </is>
       </c>
       <c r="C286" t="inlineStr">
@@ -8807,7 +8807,7 @@
       </c>
       <c r="B289" t="inlineStr">
         <is>
-          <t>@AnnaWhateley Sending hugs to the kid &amp;amp; the rest of the family</t>
+          <t>@AnnaWhateley Sending hugs to the kid &amp; the rest of the family</t>
         </is>
       </c>
       <c r="C289" t="inlineStr">
@@ -8836,7 +8836,7 @@
       </c>
       <c r="B290" t="inlineStr">
         <is>
-          <t>Poor kid has it again now, but doesn't live at home any more (I'm still dropping off food &amp;amp; meds)</t>
+          <t>Poor kid has it again now, but doesn't live at home any more (I'm still dropping off food &amp; meds)</t>
         </is>
       </c>
       <c r="C290" t="inlineStr">
@@ -8894,7 +8894,7 @@
       </c>
       <c r="B292" t="inlineStr">
         <is>
-          <t>@AnnaWhateley I left food outside the bedroom door, knocked &amp;amp; left, then they opened the door (masked) to pick it up.</t>
+          <t>@AnnaWhateley I left food outside the bedroom door, knocked &amp; left, then they opened the door (masked) to pick it up.</t>
         </is>
       </c>
       <c r="C292" t="inlineStr">
@@ -9185,7 +9185,7 @@
       </c>
       <c r="B302" t="inlineStr">
         <is>
-          <t>(Appreciate that risk &amp;amp; risk tolerance varies and understand that approach isn't for everyone)</t>
+          <t>(Appreciate that risk &amp; risk tolerance varies and understand that approach isn't for everyone)</t>
         </is>
       </c>
       <c r="C302" t="inlineStr">
@@ -10316,7 +10316,7 @@
       </c>
       <c r="B341" t="inlineStr">
         <is>
-          <t>@AnnaWhateley @sandybarker My 9 yo &amp;amp; my husband both had it a couple of weeks ago.</t>
+          <t>@AnnaWhateley @sandybarker My 9 yo &amp; my husband both had it a couple of weeks ago.</t>
         </is>
       </c>
       <c r="C341" t="inlineStr">
@@ -10925,7 +10925,7 @@
       </c>
       <c r="B362" t="inlineStr">
         <is>
-          <t>@AnnaWhateley Also, he home schooled the day before &amp;amp; sat near me all day unmasked.</t>
+          <t>@AnnaWhateley Also, he home schooled the day before &amp; sat near me all day unmasked.</t>
         </is>
       </c>
       <c r="C362" t="inlineStr">
@@ -11476,7 +11476,7 @@
       </c>
       <c r="B381" t="inlineStr">
         <is>
-          <t>Next to cancer &amp;amp; 9/11.</t>
+          <t>Next to cancer &amp; 9/11.</t>
         </is>
       </c>
       <c r="C381" t="inlineStr">
@@ -11650,7 +11650,7 @@
       </c>
       <c r="B387" t="inlineStr">
         <is>
-          <t>Covid was bad when it first got here &amp;amp; I get they panicked but that went on way too long.</t>
+          <t>Covid was bad when it first got here &amp; I get they panicked but that went on way too long.</t>
         </is>
       </c>
       <c r="C387" t="inlineStr">
@@ -15141,7 +15141,7 @@
       </c>
       <c r="B507" t="inlineStr">
         <is>
-          <t>I hope all those in #Brighton &amp;amp; #Hove got the results they were hoping for today @BHASVIC @varndean @BrightonMETcoll  #resultsday</t>
+          <t>I hope all those in #Brighton &amp; #Hove got the results they were hoping for today @BHASVIC @varndean @BrightonMETcoll  #resultsday</t>
         </is>
       </c>
       <c r="C507" t="inlineStr">
@@ -15170,7 +15170,7 @@
       </c>
       <c r="B508" t="inlineStr">
         <is>
-          <t>If education were measured by courage &amp;amp; determination shown in the face of #Covid disruption, then students  this year would pass with flying colours.</t>
+          <t>If education were measured by courage &amp; determination shown in the face of #Covid disruption, then students  this year would pass with flying colours.</t>
         </is>
       </c>
       <c r="C508" t="inlineStr">
@@ -16040,7 +16040,7 @@
       </c>
       <c r="B538" t="inlineStr">
         <is>
-          <t>I meet criteria for both hyperacusis &amp;amp; misophonia.</t>
+          <t>I meet criteria for both hyperacusis &amp; misophonia.</t>
         </is>
       </c>
       <c r="C538" t="inlineStr">
@@ -17809,7 +17809,7 @@
       </c>
       <c r="B599" t="inlineStr">
         <is>
-          <t>@catladyactivist Leaf blowers cause my inner abdominal/ torso parts to feel like they are having a massive &amp;amp; continuous earthquake.</t>
+          <t>@catladyactivist Leaf blowers cause my inner abdominal/ torso parts to feel like they are having a massive &amp; continuous earthquake.</t>
         </is>
       </c>
       <c r="C599" t="inlineStr">
@@ -18215,7 +18215,7 @@
       </c>
       <c r="B613" t="inlineStr">
         <is>
-          <t>I have 7 dogs &amp;amp; an illegal breeder in my immediate area.</t>
+          <t>I have 7 dogs &amp; an illegal breeder in my immediate area.</t>
         </is>
       </c>
       <c r="C613" t="inlineStr">
@@ -19520,7 +19520,7 @@
       </c>
       <c r="B658" t="inlineStr">
         <is>
-          <t>That they also undermine science, their credibility, truth, people’s lives &amp;amp; public health is mere collateral damage.</t>
+          <t>That they also undermine science, their credibility, truth, people’s lives &amp; public health is mere collateral damage.</t>
         </is>
       </c>
       <c r="C658" t="inlineStr">
@@ -20564,7 +20564,7 @@
       </c>
       <c r="B694" t="inlineStr">
         <is>
-          <t>Calling my electeds &amp;amp; demanding they take action.</t>
+          <t>Calling my electeds &amp; demanding they take action.</t>
         </is>
       </c>
       <c r="C694" t="inlineStr">
@@ -21087,7 +21087,7 @@
       </c>
       <c r="B712" t="inlineStr">
         <is>
-          <t>@myrabatchelder Today I’m emailing the Senators who I feel are most likely to actually care about the ongoing #covid19 pandemic, the intersectional nature of it, &amp;amp; the dark money groups behind the manufactured anti-mask sentiment.</t>
+          <t>@myrabatchelder Today I’m emailing the Senators who I feel are most likely to actually care about the ongoing #covid19 pandemic, the intersectional nature of it, &amp; the dark money groups behind the manufactured anti-mask sentiment.</t>
         </is>
       </c>
       <c r="C712" t="inlineStr">
@@ -21783,7 +21783,7 @@
       </c>
       <c r="B736" t="inlineStr">
         <is>
-          <t>It mutated bc it had no problem finding hosts as it it infected those who were (&amp;amp; still remain?)</t>
+          <t>It mutated bc it had no problem finding hosts as it it infected those who were (&amp; still remain?)</t>
         </is>
       </c>
       <c r="C736" t="inlineStr">
@@ -22334,7 +22334,7 @@
       </c>
       <c r="B755" t="inlineStr">
         <is>
-          <t>When you’re supposed to travel to #Mestia &amp;amp; finally do the Mestia-Ushguli hike, but instead test positive for #Covid in the morning 😭.</t>
+          <t>When you’re supposed to travel to #Mestia &amp; finally do the Mestia-Ushguli hike, but instead test positive for #Covid in the morning 😭.</t>
         </is>
       </c>
       <c r="C755" t="inlineStr">
@@ -23437,7 +23437,7 @@
       </c>
       <c r="B793" t="inlineStr">
         <is>
-          <t>It's toxic to see Public Health (@CDCgov) promoting individualism, marginalizing the vulnerable community, ignoring mass sickness &amp;amp; deaths.</t>
+          <t>It's toxic to see Public Health (@CDCgov) promoting individualism, marginalizing the vulnerable community, ignoring mass sickness &amp; deaths.</t>
         </is>
       </c>
       <c r="C793" t="inlineStr">
@@ -24220,7 +24220,7 @@
       </c>
       <c r="B820" t="inlineStr">
         <is>
-          <t>my mom is 80 &amp;amp; he's 91.</t>
+          <t>my mom is 80 &amp; he's 91.</t>
         </is>
       </c>
       <c r="C820" t="inlineStr">
@@ -25496,7 +25496,7 @@
       </c>
       <c r="B864" t="inlineStr">
         <is>
-          <t>Works independently of immune system status &amp;amp; we don't need others to take too, for us to have solid protection.</t>
+          <t>Works independently of immune system status &amp; we don't need others to take too, for us to have solid protection.</t>
         </is>
       </c>
       <c r="C864" t="inlineStr">
@@ -26221,7 +26221,7 @@
       </c>
       <c r="B889" t="inlineStr">
         <is>
-          <t>My heart goes out to all those experiencing iatrogenic injuries &amp;amp; medical gaslighting.</t>
+          <t>My heart goes out to all those experiencing iatrogenic injuries &amp; medical gaslighting.</t>
         </is>
       </c>
       <c r="C889" t="inlineStr">
@@ -26513,7 +26513,7 @@
       </c>
       <c r="B899" t="inlineStr">
         <is>
-          <t>@angryhacademic Further methodologically robust investigations / studies are necessary, the only way to gain reliable insights into possible causes of Long COVID &amp;amp; Post-COVID-19 reactions related to as POST-VAC SYNDROME after COVID-19 vaccination, WHICH HAS VERY SIMILAR SYMPTOMS to LONG COVID
+          <t>@angryhacademic Further methodologically robust investigations / studies are necessary, the only way to gain reliable insights into possible causes of Long COVID &amp; Post-COVID-19 reactions related to as POST-VAC SYNDROME after COVID-19 vaccination, WHICH HAS VERY SIMILAR SYMPTOMS to LONG COVID
 7/</t>
         </is>
       </c>
@@ -30778,7 +30778,7 @@
       </c>
       <c r="B1046" t="inlineStr">
         <is>
-          <t>One thing is for sure, ALP &amp;amp; Greens will be last.</t>
+          <t>One thing is for sure, ALP &amp; Greens will be last.</t>
         </is>
       </c>
       <c r="C1046" t="inlineStr">
@@ -32261,7 +32261,7 @@
       </c>
       <c r="B1097" t="inlineStr">
         <is>
-          <t>Thank you for your wise, stable &amp;amp; compassionate leadership during the pandemic.</t>
+          <t>Thank you for your wise, stable &amp; compassionate leadership during the pandemic.</t>
         </is>
       </c>
       <c r="C1097" t="inlineStr">
@@ -32493,7 +32493,7 @@
       </c>
       <c r="B1105" t="inlineStr">
         <is>
-          <t>@sleepyandnumb @CASUpdate @DrLucieFilteau Pleasure to advocate for &amp;amp; support passionate, incredibly competent #Anesthesiologists such as yourself.</t>
+          <t>@sleepyandnumb @CASUpdate @DrLucieFilteau Pleasure to advocate for &amp; support passionate, incredibly competent #Anesthesiologists such as yourself.</t>
         </is>
       </c>
       <c r="C1105" t="inlineStr">
@@ -32522,7 +32522,7 @@
       </c>
       <c r="B1106" t="inlineStr">
         <is>
-          <t>So proud to have follow you grow thru residency &amp;amp; become the amazing clinician you are ❤️💯 Just sayin.</t>
+          <t>So proud to have follow you grow thru residency &amp; become the amazing clinician you are ❤️💯 Just sayin.</t>
         </is>
       </c>
       <c r="C1106" t="inlineStr">
@@ -32551,7 +32551,7 @@
       </c>
       <c r="B1107" t="inlineStr">
         <is>
-          <t>You can give me &amp;amp; mine an anesthetic ANY day!</t>
+          <t>You can give me &amp; mine an anesthetic ANY day!</t>
         </is>
       </c>
       <c r="C1107" t="inlineStr">
@@ -32609,7 +32609,7 @@
       </c>
       <c r="B1109" t="inlineStr">
         <is>
-          <t>You are so missed my friend &amp;amp; ex-work hubby.</t>
+          <t>You are so missed my friend &amp; ex-work hubby.</t>
         </is>
       </c>
       <c r="C1109" t="inlineStr">
@@ -32812,7 +32812,7 @@
       </c>
       <c r="B1116" t="inlineStr">
         <is>
-          <t>@AnaSjaus @CASUpdate @DrLucieFilteau Kind words from an equally amazing colleague, leader, researcher &amp;amp; importantly, a valued friend ❤️🙏🏻</t>
+          <t>@AnaSjaus @CASUpdate @DrLucieFilteau Kind words from an equally amazing colleague, leader, researcher &amp; importantly, a valued friend ❤️🙏🏻</t>
         </is>
       </c>
       <c r="C1116" t="inlineStr">
@@ -33218,7 +33218,7 @@
       </c>
       <c r="B1130" t="inlineStr">
         <is>
-          <t>@AnaSjaus @CASUpdate @DrLucieFilteau Such kind words from an amazing leader, clinician &amp;amp; researcher herself.</t>
+          <t>@AnaSjaus @CASUpdate @DrLucieFilteau Such kind words from an amazing leader, clinician &amp; researcher herself.</t>
         </is>
       </c>
       <c r="C1130" t="inlineStr">
@@ -33334,7 +33334,7 @@
       </c>
       <c r="B1134" t="inlineStr">
         <is>
-          <t>Since I do not run central air am I good just sealing door and opening basement &amp;amp; main floor windows?</t>
+          <t>Since I do not run central air am I good just sealing door and opening basement &amp; main floor windows?</t>
         </is>
       </c>
       <c r="C1134" t="inlineStr">
@@ -34436,7 +34436,7 @@
       </c>
       <c r="B1172" t="inlineStr">
         <is>
-          <t>#Andrews &amp;amp; his botched #pandemic response: #Hotel #Quarantine 801 deaths, #Andrews amnesia, school &amp;amp; playground, border closures.</t>
+          <t>#Andrews &amp; his botched #pandemic response: #Hotel #Quarantine 801 deaths, #Andrews amnesia, school &amp; playground, border closures.</t>
         </is>
       </c>
       <c r="C1172" t="inlineStr">
@@ -35161,7 +35161,7 @@
       </c>
       <c r="B1197" t="inlineStr">
         <is>
-          <t>@ANCALERTS No. of cases appear to be moving on a downward trend, but ICU &amp;amp; HCU are going up.</t>
+          <t>@ANCALERTS No. of cases appear to be moving on a downward trend, but ICU &amp; HCU are going up.</t>
         </is>
       </c>
       <c r="C1197" t="inlineStr">
@@ -35741,7 +35741,7 @@
       </c>
       <c r="B1217" t="inlineStr">
         <is>
-          <t>Also would mean that anyone with would still have to report it (which they don't) - so unless people do all Test &amp;amp; Report then there are no stats!</t>
+          <t>Also would mean that anyone with would still have to report it (which they don't) - so unless people do all Test &amp; Report then there are no stats!</t>
         </is>
       </c>
       <c r="C1217" t="inlineStr">
@@ -36060,7 +36060,7 @@
       </c>
       <c r="B1228" t="inlineStr">
         <is>
-          <t>My son works in Vancouver at a popular restaurant, &amp;amp; relies on his earning &amp;amp; tips to live &amp;amp; pay rent!!!</t>
+          <t>My son works in Vancouver at a popular restaurant, &amp; relies on his earning &amp; tips to live &amp; pay rent!!!</t>
         </is>
       </c>
       <c r="C1228" t="inlineStr">
@@ -36785,7 +36785,7 @@
       </c>
       <c r="B1253" t="inlineStr">
         <is>
-          <t>As an entrepreneur who’s been self employed since 1994, I’m familiar with the vast differences between the public &amp;amp; private sectors.</t>
+          <t>As an entrepreneur who’s been self employed since 1994, I’m familiar with the vast differences between the public &amp; private sectors.</t>
         </is>
       </c>
       <c r="C1253" t="inlineStr">
@@ -37220,7 +37220,7 @@
       </c>
       <c r="B1268" t="inlineStr">
         <is>
-          <t>As a server, my son &amp;amp; thousands of workers like him are negatively impacted, and it’s “real life” for them just as much.</t>
+          <t>As a server, my son &amp; thousands of workers like him are negatively impacted, and it’s “real life” for them just as much.</t>
         </is>
       </c>
       <c r="C1268" t="inlineStr">
@@ -37249,7 +37249,7 @@
       </c>
       <c r="B1269" t="inlineStr">
         <is>
-          <t>Restaurants and their staff who rely on earnings &amp;amp; tips to pay rent, save for tuition, buy groceries, raise a family, and most with no job security, benefits, dental coverage, paid vacation time or pensions!</t>
+          <t>Restaurants and their staff who rely on earnings &amp; tips to pay rent, save for tuition, buy groceries, raise a family, and most with no job security, benefits, dental coverage, paid vacation time or pensions!</t>
         </is>
       </c>
       <c r="C1269" t="inlineStr">
@@ -37539,7 +37539,7 @@
       </c>
       <c r="B1279" t="inlineStr">
         <is>
-          <t>@jodyvance @bcgeu @BCRFA Union folks don’t understand the entrepreneurial spirit &amp;amp; risk of small business owners.</t>
+          <t>@jodyvance @bcgeu @BCRFA Union folks don’t understand the entrepreneurial spirit &amp; risk of small business owners.</t>
         </is>
       </c>
       <c r="C1279" t="inlineStr">
@@ -39656,7 +39656,7 @@
       </c>
       <c r="B1352" t="inlineStr">
         <is>
-          <t>Only fatigue &amp;amp; slight cough.</t>
+          <t>Only fatigue &amp; slight cough.</t>
         </is>
       </c>
       <c r="C1352" t="inlineStr">
@@ -44007,7 +44007,7 @@
       </c>
       <c r="B1502" t="inlineStr">
         <is>
-          <t>Spike Proteins are toxic to humans &amp;amp; are rumoured to cause long covid.</t>
+          <t>Spike Proteins are toxic to humans &amp; are rumoured to cause long covid.</t>
         </is>
       </c>
       <c r="C1502" t="inlineStr">
@@ -44036,7 +44036,7 @@
       </c>
       <c r="B1503" t="inlineStr">
         <is>
-          <t>Spike Proteins are toxic to humans &amp;amp; are rumoured to cause long covid.</t>
+          <t>Spike Proteins are toxic to humans &amp; are rumoured to cause long covid.</t>
         </is>
       </c>
       <c r="C1503" t="inlineStr">
@@ -44065,7 +44065,7 @@
       </c>
       <c r="B1504" t="inlineStr">
         <is>
-          <t>Spike Proteins are toxic to humans &amp;amp; are rumoured to cause long covid.</t>
+          <t>Spike Proteins are toxic to humans &amp; are rumoured to cause long covid.</t>
         </is>
       </c>
       <c r="C1504" t="inlineStr">
@@ -44094,7 +44094,7 @@
       </c>
       <c r="B1505" t="inlineStr">
         <is>
-          <t>Spike Proteins are toxic to humans &amp;amp; are rumoured to cause long covid.</t>
+          <t>Spike Proteins are toxic to humans &amp; are rumoured to cause long covid.</t>
         </is>
       </c>
       <c r="C1505" t="inlineStr">
@@ -45312,7 +45312,7 @@
       </c>
       <c r="B1547" t="inlineStr">
         <is>
-          <t>Your GP who was told that if they say anything negative about the vax they risk investigation &amp;amp; possible de-registration?</t>
+          <t>Your GP who was told that if they say anything negative about the vax they risk investigation &amp; possible de-registration?</t>
         </is>
       </c>
       <c r="C1547" t="inlineStr">
@@ -45689,7 +45689,7 @@
       </c>
       <c r="B1560" t="inlineStr">
         <is>
-          <t>Emergency use authorization is the first step in the approval process, &amp;amp; is based on only the first 3 months of clinical trial data.</t>
+          <t>Emergency use authorization is the first step in the approval process, &amp; is based on only the first 3 months of clinical trial data.</t>
         </is>
       </c>
       <c r="C1560" t="inlineStr">
@@ -45718,7 +45718,7 @@
       </c>
       <c r="B1561" t="inlineStr">
         <is>
-          <t>Pfizer didn't get full approval until 8 months after EUA, &amp;amp; Moderna was almost 1 year.</t>
+          <t>Pfizer didn't get full approval until 8 months after EUA, &amp; Moderna was almost 1 year.</t>
         </is>
       </c>
       <c r="C1561" t="inlineStr">
@@ -46385,7 +46385,7 @@
       </c>
       <c r="B1584" t="inlineStr">
         <is>
-          <t>@myrabatchelder Yes &amp;amp; unfortunately they are seeking treatment that fixes them quickly.</t>
+          <t>@myrabatchelder Yes &amp; unfortunately they are seeking treatment that fixes them quickly.</t>
         </is>
       </c>
       <c r="C1584" t="inlineStr">
@@ -46414,7 +46414,7 @@
       </c>
       <c r="B1585" t="inlineStr">
         <is>
-          <t>That it’s a job- requires advocacy, tenacity, patience &amp;amp; time.</t>
+          <t>That it’s a job- requires advocacy, tenacity, patience &amp; time.</t>
         </is>
       </c>
       <c r="C1585" t="inlineStr">
@@ -46791,7 +46791,7 @@
       </c>
       <c r="B1598" t="inlineStr">
         <is>
-          <t>After 6m wait colleagues &amp;amp; I all hoped that once in I’d be given The Treatment.</t>
+          <t>After 6m wait colleagues &amp; I all hoped that once in I’d be given The Treatment.</t>
         </is>
       </c>
       <c r="C1598" t="inlineStr">
@@ -46907,7 +46907,7 @@
       </c>
       <c r="B1602" t="inlineStr">
         <is>
-          <t>Colleagues &amp;amp; I assumed some rehab &amp;amp; meds programme &amp;amp; I’d be back in 6 weeks.</t>
+          <t>Colleagues &amp; I assumed some rehab &amp; meds programme &amp; I’d be back in 6 weeks.</t>
         </is>
       </c>
       <c r="C1602" t="inlineStr">
@@ -46965,7 +46965,7 @@
       </c>
       <c r="B1604" t="inlineStr">
         <is>
-          <t>(Note - we work in science) &amp;amp; all very sobered to realise truth.</t>
+          <t>(Note - we work in science) &amp; all very sobered to realise truth.</t>
         </is>
       </c>
       <c r="C1604" t="inlineStr">
@@ -47140,7 +47140,7 @@
       </c>
       <c r="B1610" t="inlineStr">
         <is>
-          <t>chix/Turkey &amp;amp; other meats some days =nausea+indigestion.</t>
+          <t>chix/Turkey &amp; other meats some days =nausea+indigestion.</t>
         </is>
       </c>
       <c r="C1610" t="inlineStr">
@@ -47576,7 +47576,7 @@
       </c>
       <c r="B1625" t="inlineStr">
         <is>
-          <t>When #COVID19 #vaccines first became avail, some decided to wait &amp;amp; see on safety.</t>
+          <t>When #COVID19 #vaccines first became avail, some decided to wait &amp; see on safety.</t>
         </is>
       </c>
       <c r="C1625" t="inlineStr">
@@ -47605,7 +47605,7 @@
       </c>
       <c r="B1626" t="inlineStr">
         <is>
-          <t>More than 12.5 BILLION doses have been given globally, &amp;amp; safety has been excellent.</t>
+          <t>More than 12.5 BILLION doses have been given globally, &amp; safety has been excellent.</t>
         </is>
       </c>
       <c r="C1626" t="inlineStr">
@@ -48360,7 +48360,7 @@
       </c>
       <c r="B1652" t="inlineStr">
         <is>
-          <t>Worth a try as anti-Hs &amp;amp; LF available online or OTC https://t.co/TGBUGBy3zS</t>
+          <t>Worth a try as anti-Hs &amp; LF available online or OTC https://t.co/TGBUGBy3zS</t>
         </is>
       </c>
       <c r="C1652" t="inlineStr">
@@ -49288,7 +49288,7 @@
       </c>
       <c r="B1684" t="inlineStr">
         <is>
-          <t>@ELHopkins I have done &amp;amp; complained to the Chief Exec, Infection Control &amp;amp; PALS.</t>
+          <t>@ELHopkins I have done &amp; complained to the Chief Exec, Infection Control &amp; PALS.</t>
         </is>
       </c>
       <c r="C1684" t="inlineStr">
@@ -49578,7 +49578,7 @@
       </c>
       <c r="B1694" t="inlineStr">
         <is>
-          <t>@VeniceLaura @ELHopkins Royal Berkshire Hospital (local A&amp;amp;E) don't have a mask policy... the hospital where I'm treated for my RA, the Nuffield Orthopaedic Centre does.</t>
+          <t>@VeniceLaura @ELHopkins Royal Berkshire Hospital (local A&amp;E) don't have a mask policy... the hospital where I'm treated for my RA, the Nuffield Orthopaedic Centre does.</t>
         </is>
       </c>
       <c r="C1694" t="inlineStr">
@@ -53446,7 +53446,7 @@
       </c>
       <c r="B1827" t="inlineStr">
         <is>
-          <t>I work retail, &amp;amp; never wear a mask except on an airplane.</t>
+          <t>I work retail, &amp; never wear a mask except on an airplane.</t>
         </is>
       </c>
       <c r="C1827" t="inlineStr">
@@ -55274,7 +55274,7 @@
       </c>
       <c r="B1890" t="inlineStr">
         <is>
-          <t>@ELHopkins @drcarolinej is both my MP &amp;amp; a paediatrician yet still votes against mitigations in schools &amp;amp; society generally.</t>
+          <t>@ELHopkins @drcarolinej is both my MP &amp; a paediatrician yet still votes against mitigations in schools &amp; society generally.</t>
         </is>
       </c>
       <c r="C1890" t="inlineStr">
@@ -55303,7 +55303,7 @@
       </c>
       <c r="B1891" t="inlineStr">
         <is>
-          <t>She very obviously takes her duty of care towards her constituents &amp;amp; society extremely seriously (sarcasm intended).</t>
+          <t>She very obviously takes her duty of care towards her constituents &amp; society extremely seriously (sarcasm intended).</t>
         </is>
       </c>
       <c r="C1891" t="inlineStr">
@@ -55419,7 +55419,7 @@
       </c>
       <c r="B1895" t="inlineStr">
         <is>
-          <t>Their attitude is disgusting &amp;amp; criminal IMO.</t>
+          <t>Their attitude is disgusting &amp; criminal IMO.</t>
         </is>
       </c>
       <c r="C1895" t="inlineStr">
@@ -56058,7 +56058,7 @@
       <c r="B1917" t="inlineStr">
         <is>
           <t>They would’ve accepted it but I also think they would’ve stuck the machine in the corner
-&amp;amp; not used it or complained about the noise, hence I didn’t end up buying one for the school.</t>
+&amp; not used it or complained about the noise, hence I didn’t end up buying one for the school.</t>
         </is>
       </c>
       <c r="C1917" t="inlineStr">
@@ -56377,7 +56377,7 @@
       </c>
       <c r="B1928" t="inlineStr">
         <is>
-          <t>@PatCrosbie1 @ELHopkins The latest information from the ONS for England &amp;amp; Wales covers 2020, but that was the height of the “pandemic”.</t>
+          <t>@PatCrosbie1 @ELHopkins The latest information from the ONS for England &amp; Wales covers 2020, but that was the height of the “pandemic”.</t>
         </is>
       </c>
       <c r="C1928" t="inlineStr">
@@ -56464,7 +56464,7 @@
       </c>
       <c r="B1931" t="inlineStr">
         <is>
-          <t>There are 11.4 million children aged 0-15 in England &amp;amp; Wales. https://t.co/CCJI5cyToH</t>
+          <t>There are 11.4 million children aged 0-15 in England &amp; Wales. https://t.co/CCJI5cyToH</t>
         </is>
       </c>
       <c r="C1931" t="inlineStr">
@@ -56727,7 +56727,7 @@
       </c>
       <c r="B1940" t="inlineStr">
         <is>
-          <t>Australia is nearing the end of its worst flu season in 5 years &amp;amp; it could be a sign of what’s to come in the U.S. this year.</t>
+          <t>Australia is nearing the end of its worst flu season in 5 years &amp; it could be a sign of what’s to come in the U.S. this year.</t>
         </is>
       </c>
       <c r="C1940" t="inlineStr">
@@ -57946,7 +57946,7 @@
       </c>
       <c r="B1982" t="inlineStr">
         <is>
-          <t>Elevated heart rate, respiration, &amp;amp; strained recovery similar to having run a marathon 1/x https://t.co/xE1fP5DYnh</t>
+          <t>Elevated heart rate, respiration, &amp; strained recovery similar to having run a marathon 1/x https://t.co/xE1fP5DYnh</t>
         </is>
       </c>
       <c r="C1982" t="inlineStr">
@@ -57975,7 +57975,7 @@
       </c>
       <c r="B1983" t="inlineStr">
         <is>
-          <t>I’m vaxxed &amp;amp; double boosted, healthy.</t>
+          <t>I’m vaxxed &amp; double boosted, healthy.</t>
         </is>
       </c>
       <c r="C1983" t="inlineStr">
@@ -58062,7 +58062,7 @@
       </c>
       <c r="B1986" t="inlineStr">
         <is>
-          <t>In the run up to this, I’ve been actually feeling in great shape/fitness as I train for the #JFK50 &amp;amp; #MCM50k.</t>
+          <t>In the run up to this, I’ve been actually feeling in great shape/fitness as I train for the #JFK50 &amp; #MCM50k.</t>
         </is>
       </c>
       <c r="C1986" t="inlineStr">
@@ -60618,7 +60618,7 @@
       </c>
       <c r="B2074" t="inlineStr">
         <is>
-          <t>The suicide rate has not increased &amp;amp; has actually gone down during the pandemic in some places.</t>
+          <t>The suicide rate has not increased &amp; has actually gone down during the pandemic in some places.</t>
         </is>
       </c>
       <c r="C2074" t="inlineStr">
@@ -61838,7 +61838,7 @@
       </c>
       <c r="B2116" t="inlineStr">
         <is>
-          <t>@CVinjured I would stop &amp;amp; help!</t>
+          <t>@CVinjured I would stop &amp; help!</t>
         </is>
       </c>
       <c r="C2116" t="inlineStr">
@@ -62391,7 +62391,7 @@
       </c>
       <c r="B2135" t="inlineStr">
         <is>
-          <t>Country after country exhibited an unusual &amp;amp; for the summertime quite extreme number of deaths, larger than even previous two summers, yet it supposedly somehow can be explained by aging population but not #COVID.</t>
+          <t>Country after country exhibited an unusual &amp; for the summertime quite extreme number of deaths, larger than even previous two summers, yet it supposedly somehow can be explained by aging population but not #COVID.</t>
         </is>
       </c>
       <c r="C2135" t="inlineStr">
@@ -66077,7 +66077,7 @@
       </c>
       <c r="B2262" t="inlineStr">
         <is>
-          <t>How is PCR "fake" &amp;amp; what is your experience with it.</t>
+          <t>How is PCR "fake" &amp; what is your experience with it.</t>
         </is>
       </c>
       <c r="C2262" t="inlineStr">
@@ -66338,7 +66338,7 @@
       </c>
       <c r="B2271" t="inlineStr">
         <is>
-          <t>But those that keep saying that it has no side effects &amp;amp; is not bad at all, is the issue w/ those numbnuts on here.</t>
+          <t>But those that keep saying that it has no side effects &amp; is not bad at all, is the issue w/ those numbnuts on here.</t>
         </is>
       </c>
       <c r="C2271" t="inlineStr">
@@ -66715,7 +66715,7 @@
       </c>
       <c r="B2284" t="inlineStr">
         <is>
-          <t>Like I tell others, go to my social media and follow my time before the jab &amp;amp; after.</t>
+          <t>Like I tell others, go to my social media and follow my time before the jab &amp; after.</t>
         </is>
       </c>
       <c r="C2284" t="inlineStr">
@@ -67208,7 +67208,7 @@
       </c>
       <c r="B2301" t="inlineStr">
         <is>
-          <t>But don't take my word for it, go to VAERS &amp;amp; the European system and look at the info reported on all of the adverse reactions.</t>
+          <t>But don't take my word for it, go to VAERS &amp; the European system and look at the info reported on all of the adverse reactions.</t>
         </is>
       </c>
       <c r="C2301" t="inlineStr">
@@ -70343,7 +70343,7 @@
       </c>
       <c r="B2409" t="inlineStr">
         <is>
-          <t>i too suffer from allergies 🤧 some have suggested a connection between #LongCovid &amp;amp; atopy..</t>
+          <t>i too suffer from allergies 🤧 some have suggested a connection between #LongCovid &amp; atopy..</t>
         </is>
       </c>
       <c r="C2409" t="inlineStr">
@@ -70749,7 +70749,7 @@
       </c>
       <c r="B2423" t="inlineStr">
         <is>
-          <t>i guess the real question is do you expect the rapid to give you a fair &amp;amp; accurate reading?</t>
+          <t>i guess the real question is do you expect the rapid to give you a fair &amp; accurate reading?</t>
         </is>
       </c>
       <c r="C2423" t="inlineStr">
@@ -72518,7 +72518,7 @@
       </c>
       <c r="B2484" t="inlineStr">
         <is>
-          <t>hopefully they keep feeling better &amp;amp; better https://t.co/9c3y4FFtce</t>
+          <t>hopefully they keep feeling better &amp; better https://t.co/9c3y4FFtce</t>
         </is>
       </c>
       <c r="C2484" t="inlineStr">

</xml_diff>